<commit_message>
refactor: move excel writer to visualize_data
</commit_message>
<xml_diff>
--- a/PH_SAM.xlsx
+++ b/PH_SAM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vince\OneDrive\Documents\CS 199\CGE\open_cge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University of the Philippines\4th Year 2nd Sem (4.2) LAST SEM!\CS 199\CGE_Ipopt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B0C64B-6B3D-4313-BEE2-2B223EC9A5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730D71D0-5C58-4686-9A53-FEA583BF7410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{64C2337D-9F83-4F1D-B26B-0C6F79C1C225}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{64C2337D-9F83-4F1D-B26B-0C6F79C1C225}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,10 +134,47 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -146,8 +183,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,91 +524,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657EFB9F-0A0A-40F6-9343-279823100FC5}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="J16" workbookViewId="0">
+      <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -643,12 +684,12 @@
       <c r="Y2">
         <v>88379.20989359371</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="3">
         <v>3539337.012263726</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -723,12 +764,12 @@
       <c r="Y3">
         <v>80038.600741612201</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="3">
         <v>562958.43174198852</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -803,12 +844,12 @@
       <c r="Y4">
         <v>2920941.7587366384</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="3">
         <v>16750930.285265801</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -883,12 +924,12 @@
       <c r="Y5">
         <v>0.17079307186492348</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="3">
         <v>897254.57100810169</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6">
@@ -963,12 +1004,12 @@
       <c r="Y6">
         <v>3019.3613223447037</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="3">
         <v>3012061.5757628679</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7">
@@ -1043,12 +1084,12 @@
       <c r="Y7">
         <v>302312.19112610229</v>
       </c>
-      <c r="Z7">
+      <c r="Z7" s="3">
         <v>4686043.3527094247</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -1123,12 +1164,12 @@
       <c r="Y8">
         <v>339911.89130274311</v>
       </c>
-      <c r="Z8">
+      <c r="Z8" s="3">
         <v>2005437.9784490601</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -1203,12 +1244,12 @@
       <c r="Y9">
         <v>467265.75904066919</v>
       </c>
-      <c r="Z9">
+      <c r="Z9" s="3">
         <v>1714934.5570438774</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10">
@@ -1283,12 +1324,12 @@
       <c r="Y10">
         <v>303862.50513532205</v>
       </c>
-      <c r="Z10">
+      <c r="Z10" s="3">
         <v>1122902.3435364489</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11">
@@ -1363,12 +1404,12 @@
       <c r="Y11">
         <v>44667.503055926049</v>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="3">
         <v>2863978.1498217527</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B12">
@@ -1443,12 +1484,12 @@
       <c r="Y12">
         <v>6203.6046702851199</v>
       </c>
-      <c r="Z12">
+      <c r="Z12" s="3">
         <v>1656695.3834001769</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B13">
@@ -1523,12 +1564,12 @@
       <c r="Y13">
         <v>839824.06285198231</v>
       </c>
-      <c r="Z13">
+      <c r="Z13" s="3">
         <v>2125070.1371444552</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B14">
@@ -1603,12 +1644,12 @@
       <c r="Y14">
         <v>10181.819916173105</v>
       </c>
-      <c r="Z14">
+      <c r="Z14" s="3">
         <v>1293539.4771354618</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B15">
@@ -1683,12 +1724,12 @@
       <c r="Y15">
         <v>62709.115267949739</v>
       </c>
-      <c r="Z15">
+      <c r="Z15" s="3">
         <v>869326.07469321659</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B16">
@@ -1763,12 +1804,12 @@
       <c r="Y16">
         <v>8969.8095543311974</v>
       </c>
-      <c r="Z16">
+      <c r="Z16" s="3">
         <v>466372.66667972429</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17">
@@ -1843,12 +1884,12 @@
       <c r="Y17">
         <v>40285.141883514167</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="3">
         <v>634839.1190750252</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18">
@@ -1923,12 +1964,12 @@
       <c r="Y18">
         <v>0</v>
       </c>
-      <c r="Z18">
+      <c r="Z18" s="3">
         <v>10583750.258161744</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19">
@@ -2003,12 +2044,12 @@
       <c r="Y19">
         <v>0</v>
       </c>
-      <c r="Z19">
+      <c r="Z19" s="3">
         <v>6297084</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B20">
@@ -2083,12 +2124,12 @@
       <c r="Y20">
         <v>0</v>
       </c>
-      <c r="Z20">
+      <c r="Z20" s="3">
         <v>1384356</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B21">
@@ -2163,12 +2204,12 @@
       <c r="Y21">
         <v>0</v>
       </c>
-      <c r="Z21">
+      <c r="Z21" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B22">
@@ -2243,12 +2284,12 @@
       <c r="Y22">
         <v>0</v>
       </c>
-      <c r="Z22">
+      <c r="Z22" s="3">
         <v>16880834.258161746</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B23">
@@ -2323,12 +2364,12 @@
       <c r="Y23">
         <v>0</v>
       </c>
-      <c r="Z23">
+      <c r="Z23" s="3">
         <v>2329625.9536134987</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B24">
@@ -2403,12 +2444,12 @@
       <c r="Y24">
         <v>2143636.985557205</v>
       </c>
-      <c r="Z24">
+      <c r="Z24" s="3">
         <v>4959105.4661447657</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B25">
@@ -2483,88 +2524,90 @@
       <c r="Y25">
         <v>0</v>
       </c>
-      <c r="Z25">
+      <c r="Z25" s="3">
         <v>7662209.4908494642</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>3539337.0030186493</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>562958.43039211398</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>16750930.245826636</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>897254.5689391651</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>3012061.6717931968</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <v>4686043.3419791451</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="1">
         <v>2005437.9738954324</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="1">
         <v>1714934.553139891</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="1">
         <v>1122902.3410094911</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="1">
         <v>2863978.1432694099</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="1">
         <v>1656695.3798830861</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="1">
         <v>2125070.1323891641</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="1">
         <v>1293539.4741678732</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="1">
         <v>869326.07274930901</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="1">
         <v>466372.66563166049</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="1">
         <v>634839.1176468851</v>
       </c>
-      <c r="R26">
+      <c r="R26" s="1">
         <v>10583750.258161744</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="1">
         <v>6297084</v>
       </c>
-      <c r="T26">
+      <c r="T26" s="1">
         <v>1384356</v>
       </c>
-      <c r="U26">
-        <v>0</v>
-      </c>
-      <c r="V26">
+      <c r="U26" s="1">
+        <v>0</v>
+      </c>
+      <c r="V26" s="1">
         <v>16880834.258161746</v>
       </c>
-      <c r="W26">
+      <c r="W26" s="1">
         <v>2329625.9536134987</v>
       </c>
-      <c r="X26">
+      <c r="X26" s="1">
         <v>4959105.4661447704</v>
       </c>
-      <c r="Y26">
+      <c r="Y26" s="1">
         <v>7662209.4908494642</v>
       </c>
+      <c r="Z26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>